<commit_message>
Fixed the upload file, added exporting files; SQL: added change_nmber_stock_bulk (Might delete later tho)
</commit_message>
<xml_diff>
--- a/backend/vg_data__1.xlsx
+++ b/backend/vg_data__1.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B7FF4B-DECE-4F36-B0BD-E0957E31491D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-330" yWindow="3780" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" windowHeight="15345" windowWidth="28800" xWindow="-330" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="3780"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -83,17 +83,36 @@
   <si>
     <t>New Super Mario Bros. Wii</t>
   </si>
+  <si>
+    <t>Item_idName</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Barcode</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" count="8" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="8">
+    <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);(&quot;$&quot;#,##0)"/>
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red](&quot;$&quot;#,##0)"/>
+    <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00_);(&quot;$&quot;#,##0.00)"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red](&quot;$&quot;#,##0.00)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* (#,##0);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* (#,##0);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* (#,##0.00);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* (#,##0.00);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -107,15 +126,25 @@
   </fills>
   <borders count="1">
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -398,34 +427,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView workbookViewId="0" tabSelected="1">
+      <selection pane="topLeft" activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
+      <c r="A1" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>21</v>
       </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -433,16 +464,16 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="C2">
-        <v>82</v>
-      </c>
-      <c r="D2">
+      <c r="D2" s="0">
+        <v>1</v>
+      </c>
+      <c r="E2">
         <v>40</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -450,16 +481,16 @@
       <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="C3">
-        <v>40</v>
-      </c>
-      <c r="D3">
+      <c r="D3" s="0">
+        <v>1</v>
+      </c>
+      <c r="E3">
         <v>20</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>7</v>
       </c>
     </row>
@@ -467,16 +498,16 @@
       <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>6</v>
       </c>
-      <c r="C4">
-        <v>35</v>
-      </c>
-      <c r="D4">
+      <c r="D4" s="0">
+        <v>1</v>
+      </c>
+      <c r="E4">
         <v>40</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -484,16 +515,16 @@
       <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>6</v>
       </c>
-      <c r="C5">
-        <v>33</v>
-      </c>
-      <c r="D5">
+      <c r="D5" s="0">
+        <v>1</v>
+      </c>
+      <c r="E5">
         <v>40</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>7</v>
       </c>
     </row>
@@ -501,16 +532,16 @@
       <c r="A6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>13</v>
       </c>
-      <c r="C6">
-        <v>31</v>
-      </c>
-      <c r="D6">
+      <c r="D6" s="0">
+        <v>1</v>
+      </c>
+      <c r="E6">
         <v>20</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>7</v>
       </c>
     </row>
@@ -518,16 +549,16 @@
       <c r="A7" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>13</v>
       </c>
-      <c r="C7">
-        <v>30</v>
-      </c>
-      <c r="D7">
+      <c r="D7" s="0">
+        <v>1</v>
+      </c>
+      <c r="E7">
         <v>20</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>7</v>
       </c>
     </row>
@@ -535,16 +566,16 @@
       <c r="A8" t="s">
         <v>15</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>16</v>
       </c>
-      <c r="C8">
-        <v>30</v>
-      </c>
-      <c r="D8">
+      <c r="D8" s="0">
+        <v>1</v>
+      </c>
+      <c r="E8">
         <v>40</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>7</v>
       </c>
     </row>
@@ -552,16 +583,16 @@
       <c r="A9" t="s">
         <v>17</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>6</v>
       </c>
-      <c r="C9">
-        <v>29</v>
-      </c>
-      <c r="D9">
+      <c r="D9" s="0">
+        <v>1</v>
+      </c>
+      <c r="E9">
         <v>40</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>7</v>
       </c>
     </row>
@@ -569,16 +600,16 @@
       <c r="A10" t="s">
         <v>18</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>6</v>
       </c>
-      <c r="C10">
-        <v>28</v>
-      </c>
-      <c r="D10">
+      <c r="D10" s="0">
+        <v>1</v>
+      </c>
+      <c r="E10">
         <v>40</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>